<commit_message>
correct login depending on user's accesstype
</commit_message>
<xml_diff>
--- a/src/main/resources/database/user_account.xlsx
+++ b/src/main/resources/database/user_account.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaIDE\test\src\main\resources\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\clothing-store\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C5FA7E-779A-46BF-9BDC-FC12898C85EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675DE174-1891-4B96-B683-CEBA8D9672B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="5328" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>alina_bybko@mail.ru</t>
   </si>
@@ -85,12 +85,52 @@
   </si>
   <si>
     <t>Glebtsova</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin@mail.ru</t>
+  </si>
+  <si>
+    <t>yoda</t>
+  </si>
+  <si>
+    <t>123yoda</t>
+  </si>
+  <si>
+    <t>yoda@gmail.com</t>
+  </si>
+  <si>
+    <t>yyy</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>andrey</t>
+  </si>
+  <si>
+    <t>andrey11223344</t>
+  </si>
+  <si>
+    <t>andrin@mail.ru</t>
+  </si>
+  <si>
+    <t>Andrey</t>
+  </si>
+  <si>
+    <t>Skvortsov</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,22 +454,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A5:A7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="15.21875"/>
+    <col min="3" max="3" customWidth="true" width="15.6640625"/>
+    <col min="4" max="4" customWidth="true" width="24.21875"/>
+    <col min="5" max="5" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" customWidth="true" width="9.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -448,8 +488,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -468,8 +511,11 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -488,8 +534,11 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -507,13 +556,87 @@
       </c>
       <c r="F4" t="s">
         <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" xr:uid="{06CF7475-6F1C-4265-8137-9A45FB629F5F}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{775F3B77-9359-466B-AB3E-3E2D5535417A}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{7D6A01D1-7653-45DD-9448-B68078BE68E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>